<commit_message>
2# fechamento da primeira entraga
o termo dupla so se for de 1
</commit_message>
<xml_diff>
--- a/requisitos/UC/UC - Alocar professor a uma disciplina.xlsx
+++ b/requisitos/UC/UC - Alocar professor a uma disciplina.xlsx
@@ -36,9 +36,6 @@
     <t>Clicar na opção "Alocar Professor em uma disciplina"</t>
   </si>
   <si>
-    <t>Uma nova tela é exibida contendo as disciplinas e os professores que ainda não foram alocados</t>
-  </si>
-  <si>
     <t>Selecionar uma disciplina e um professor e logo após clicar em "Confirmar"</t>
   </si>
   <si>
@@ -61,13 +58,6 @@
   </si>
   <si>
     <t>Resultado esperado</t>
-  </si>
-  <si>
-    <t>Clicar na opção "Alocar Professor em uma disciplina" sem haver professor(es) e/ou disciplina(s) disponíveis.</t>
-  </si>
-  <si>
-    <t>É Exibida na tela uma mensagem, informando  para o administrador que não há professor(es) ou disciplina(s) suficientes para alocação.
-A operação é encerrada.</t>
   </si>
   <si>
     <t>Não selecionar uma disciplina e selecionar um professor e logo após clicar em "Confirmar"</t>
@@ -121,6 +111,16 @@
   <si>
     <t>Exibir uma mensagem para o administrador informando que selecione um item na lista.
 Volta para a opção de seleção de disciplina e professor.</t>
+  </si>
+  <si>
+    <t>Uma nova tela é exibida contendo uma lista dos professores e outra lista com as disciplinas que ainda não tem professores alocados.</t>
+  </si>
+  <si>
+    <t>É Exibida na tela uma mensagem, informando  para o administrador que não há  "Não a Disciplinas Cadastrada!! "para caso da disciplina disciplina, e para cso do professor "Não ha professor Cadastrado" 
+A operação é encerrada.</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Alocar Professor em uma disciplina" sem haver professor(es) e/ou disciplina(s) cadastrados.</t>
   </si>
 </sst>
 </file>
@@ -212,16 +212,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -540,18 +540,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -562,15 +562,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -578,10 +578,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -589,10 +589,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -600,10 +600,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -611,37 +611,37 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>15</v>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -649,18 +649,18 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#2 corração Alocar Professor
</commit_message>
<xml_diff>
--- a/requisitos/UC/UC - Alocar professor a uma disciplina.xlsx
+++ b/requisitos/UC/UC - Alocar professor a uma disciplina.xlsx
@@ -36,6 +36,9 @@
     <t>Clicar na opção "Alocar Professor em uma disciplina"</t>
   </si>
   <si>
+    <t>Uma nova tela é exibida contendo as disciplinas e os professores que ainda não foram alocados</t>
+  </si>
+  <si>
     <t>Selecionar uma disciplina e um professor e logo após clicar em "Confirmar"</t>
   </si>
   <si>
@@ -58,6 +61,13 @@
   </si>
   <si>
     <t>Resultado esperado</t>
+  </si>
+  <si>
+    <t>Clicar na opção "Alocar Professor em uma disciplina" sem haver professor(es) e/ou disciplina(s) disponíveis.</t>
+  </si>
+  <si>
+    <t>É Exibida na tela uma mensagem, informando  para o administrador que não há professor(es) ou disciplina(s) suficientes para alocação.
+A operação é encerrada.</t>
   </si>
   <si>
     <t>Não selecionar uma disciplina e selecionar um professor e logo após clicar em "Confirmar"</t>
@@ -111,16 +121,6 @@
   <si>
     <t>Exibir uma mensagem para o administrador informando que selecione um item na lista.
 Volta para a opção de seleção de disciplina e professor.</t>
-  </si>
-  <si>
-    <t>Uma nova tela é exibida contendo uma lista dos professores e outra lista com as disciplinas que ainda não tem professores alocados.</t>
-  </si>
-  <si>
-    <t>É Exibida na tela uma mensagem, informando  para o administrador que não há  "Não a Disciplinas Cadastrada!! "para caso da disciplina disciplina, e para cso do professor "Não ha professor Cadastrado" 
-A operação é encerrada.</t>
-  </si>
-  <si>
-    <t>Clicar na opção "Alocar Professor em uma disciplina" sem haver professor(es) e/ou disciplina(s) cadastrados.</t>
   </si>
 </sst>
 </file>
@@ -212,16 +212,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +529,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -540,18 +540,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -562,15 +562,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>19</v>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -578,10 +578,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -589,10 +589,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -600,10 +600,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -611,37 +611,37 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>17</v>
+        <v>10</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>20</v>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -649,18 +649,18 @@
         <v>2</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>